<commit_message>
rev after 2 feb
</commit_message>
<xml_diff>
--- a/public/file_excel/Format Plotting Dosen Pembimbing.xlsx
+++ b/public/file_excel/Format Plotting Dosen Pembimbing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\skripsi\public\file_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62AC723-273A-41E3-A7F8-1E1024479AA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF6CEE6-B0F0-4037-96F4-72796D8017A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7515" xr2:uid="{E73C28A4-EC72-4FA6-963C-AB4488427729}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>GASAL 2021/2022</t>
   </si>
@@ -33,21 +33,6 @@
     <t>NAMA MAHASISWA</t>
   </si>
   <si>
-    <t>00406107004</t>
-  </si>
-  <si>
-    <t>00406107005</t>
-  </si>
-  <si>
-    <t>00406107006</t>
-  </si>
-  <si>
-    <t>00406107007</t>
-  </si>
-  <si>
-    <t>00406107008</t>
-  </si>
-  <si>
     <t>0608068502</t>
   </si>
   <si>
@@ -61,6 +46,51 @@
   </si>
   <si>
     <t>0608068506</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>Nim</t>
+  </si>
+  <si>
+    <t>Nama</t>
+  </si>
+  <si>
+    <t>00406107055</t>
+  </si>
+  <si>
+    <t>00406107056</t>
+  </si>
+  <si>
+    <t>00406107057</t>
+  </si>
+  <si>
+    <t>00406107058</t>
+  </si>
+  <si>
+    <t>00406107059</t>
+  </si>
+  <si>
+    <t>NIDN_Dosen_Pembimbing_Utama</t>
+  </si>
+  <si>
+    <t>NIDN_Dosen_Pembimbing_Pembantu</t>
+  </si>
+  <si>
+    <t>Nama_Dosen_Pembimbing_Utama</t>
+  </si>
+  <si>
+    <t>Nama_Dosen_Pembimbing_Pembantu</t>
+  </si>
+  <si>
+    <t>Ratih Nindyasari, S.Kom, M.Kom</t>
+  </si>
+  <si>
+    <t>Anastasya Latubessy, S.Kom, M.Cs</t>
   </si>
 </sst>
 </file>
@@ -413,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7B0C3A-F3AD-494D-BA8F-A490C13DEE06}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F5"/>
+      <selection activeCell="H2" sqref="H2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,108 +454,166 @@
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="33.140625" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" customWidth="1"/>
+    <col min="7" max="7" width="37.42578125" customWidth="1"/>
+    <col min="8" max="8" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>201851001</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>201851002</v>
+        <v>201851001</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>201851003</v>
+        <v>201851002</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>201851004</v>
+        <v>201851003</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>201851005</v>
+        <v>201851004</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>201851005</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
+      <c r="H6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rev after 2 feb v3
</commit_message>
<xml_diff>
--- a/public/file_excel/Format Plotting Dosen Pembimbing.xlsx
+++ b/public/file_excel/Format Plotting Dosen Pembimbing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\skripsi\public\file_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF6CEE6-B0F0-4037-96F4-72796D8017A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFF8DC8-7D25-4D70-9FE9-AA9431F97558}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7515" xr2:uid="{E73C28A4-EC72-4FA6-963C-AB4488427729}"/>
   </bookViews>
@@ -97,8 +97,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -126,9 +134,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +455,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H6"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,29 +469,29 @@
     <col min="8" max="8" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -618,5 +627,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix : penyesuaian plotting dosen pembimbing untuk proposal
remove anomaly folder
</commit_message>
<xml_diff>
--- a/public/file_excel/Format Plotting Dosen Pembimbing.xlsx
+++ b/public/file_excel/Format Plotting Dosen Pembimbing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\skripsi\public\file_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\sistem-monitoring-skripsi\public\file_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC1E1D9-70C2-4BC0-9BAF-D861C923EAC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8014BE7C-B3B8-4249-9715-1737B0C97E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7515" xr2:uid="{E73C28A4-EC72-4FA6-963C-AB4488427729}"/>
+    <workbookView xWindow="3150" yWindow="3195" windowWidth="21600" windowHeight="11295" xr2:uid="{E73C28A4-EC72-4FA6-963C-AB4488427729}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7B0C3A-F3AD-494D-BA8F-A490C13DEE06}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>